<commit_message>
first pass plotting mobility
</commit_message>
<xml_diff>
--- a/raw_data/metadata.xlsx
+++ b/raw_data/metadata.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/joegunn/Desktop/Projects/active_projects/CPB_Phenotype/raw_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{097795A9-F79C-C445-9A2E-6BA632672BAA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{752F2F42-04DF-3745-ACAF-8F5BBE90376E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-31820" yWindow="840" windowWidth="28800" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1849,8 +1849,8 @@
   </sheetPr>
   <dimension ref="A1:X1049"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A682" workbookViewId="0">
-      <selection activeCell="G175" sqref="G175"/>
+    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="G26" sqref="G26:G169"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1"/>
@@ -2998,7 +2998,7 @@
         <v>197</v>
       </c>
       <c r="G27" s="7" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="H27" s="7" t="s">
         <v>12</v>
@@ -3072,7 +3072,7 @@
         <v>471</v>
       </c>
       <c r="G29" s="7" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="H29" s="7"/>
       <c r="I29" s="7"/>
@@ -3220,7 +3220,7 @@
         <v>285</v>
       </c>
       <c r="G33" s="7" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="H33" s="7" t="s">
         <v>12</v>
@@ -3258,7 +3258,7 @@
         <v>234</v>
       </c>
       <c r="G34" s="7" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="H34" s="7" t="s">
         <v>12</v>
@@ -3296,7 +3296,7 @@
         <v>192</v>
       </c>
       <c r="G35" s="7" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="H35" s="7" t="s">
         <v>13</v>
@@ -3410,7 +3410,7 @@
         <v>188</v>
       </c>
       <c r="G38" s="7" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="H38" s="7" t="s">
         <v>12</v>
@@ -3448,7 +3448,7 @@
         <v>472</v>
       </c>
       <c r="G39" s="7" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="H39" s="7" t="s">
         <v>12</v>
@@ -3486,7 +3486,7 @@
         <v>188</v>
       </c>
       <c r="G40" s="7" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="H40" s="7"/>
       <c r="I40" s="7"/>
@@ -3520,7 +3520,7 @@
         <v>208</v>
       </c>
       <c r="G41" s="7" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="H41" s="7" t="s">
         <v>13</v>
@@ -3594,7 +3594,7 @@
         <v>285</v>
       </c>
       <c r="G43" s="7" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="H43" s="7" t="s">
         <v>13</v>
@@ -3670,7 +3670,7 @@
         <v>211</v>
       </c>
       <c r="G45" s="7" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="H45" s="7" t="s">
         <v>13</v>
@@ -3708,7 +3708,7 @@
         <v>234</v>
       </c>
       <c r="G46" s="7" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="H46" s="7" t="s">
         <v>12</v>
@@ -3822,7 +3822,7 @@
         <v>208</v>
       </c>
       <c r="G49" s="7" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="H49" s="7" t="s">
         <v>12</v>
@@ -3860,7 +3860,7 @@
         <v>285</v>
       </c>
       <c r="G50" s="7" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="H50" s="7"/>
       <c r="I50" s="7"/>
@@ -3968,7 +3968,7 @@
         <v>211</v>
       </c>
       <c r="G53" s="7" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="H53" s="7"/>
       <c r="I53" s="7"/>
@@ -4040,7 +4040,7 @@
         <v>192</v>
       </c>
       <c r="G55" s="7" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="H55" s="7" t="s">
         <v>13</v>
@@ -4078,7 +4078,7 @@
         <v>234</v>
       </c>
       <c r="G56" s="7" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="H56" s="7" t="s">
         <v>13</v>
@@ -4114,7 +4114,7 @@
         <v>188</v>
       </c>
       <c r="G57" s="7" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="H57" s="7" t="s">
         <v>12</v>
@@ -4152,7 +4152,7 @@
         <v>471</v>
       </c>
       <c r="G58" s="7" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="H58" s="7"/>
       <c r="I58" s="7"/>
@@ -4224,7 +4224,7 @@
         <v>472</v>
       </c>
       <c r="G60" s="7" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="H60" s="7"/>
       <c r="I60" s="7"/>
@@ -4258,7 +4258,7 @@
         <v>188</v>
       </c>
       <c r="G61" s="7" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="H61" s="7"/>
       <c r="I61" s="7"/>
@@ -4406,7 +4406,7 @@
         <v>234</v>
       </c>
       <c r="G65" s="7" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="H65" s="7" t="s">
         <v>12</v>
@@ -4558,7 +4558,7 @@
         <v>472</v>
       </c>
       <c r="G69" s="7" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="H69" s="7"/>
       <c r="I69" s="7"/>
@@ -4702,7 +4702,7 @@
         <v>471</v>
       </c>
       <c r="G73" s="7" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="H73" s="7"/>
       <c r="I73" s="7"/>
@@ -4884,7 +4884,7 @@
         <v>472</v>
       </c>
       <c r="G78" s="7" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="H78" s="7" t="s">
         <v>12</v>
@@ -4920,7 +4920,7 @@
         <v>472</v>
       </c>
       <c r="G79" s="7" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="H79" s="7"/>
       <c r="I79" s="7"/>
@@ -4954,7 +4954,7 @@
         <v>472</v>
       </c>
       <c r="G80" s="7" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="H80" s="7"/>
       <c r="I80" s="7"/>
@@ -5102,7 +5102,7 @@
         <v>188</v>
       </c>
       <c r="G84" s="7" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="H84" s="7"/>
       <c r="I84" s="7"/>
@@ -5208,7 +5208,7 @@
         <v>285</v>
       </c>
       <c r="G87" s="7" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="H87" s="7"/>
       <c r="I87" s="7"/>
@@ -5280,7 +5280,7 @@
         <v>211</v>
       </c>
       <c r="G89" s="7" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="H89" s="7"/>
       <c r="I89" s="7"/>
@@ -5352,7 +5352,7 @@
         <v>208</v>
       </c>
       <c r="G91" s="7" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="H91" s="7" t="s">
         <v>13</v>
@@ -5428,7 +5428,7 @@
         <v>211</v>
       </c>
       <c r="G93" s="7" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="H93" s="7" t="s">
         <v>12</v>
@@ -5542,7 +5542,7 @@
         <v>197</v>
       </c>
       <c r="G96" s="7" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="H96" s="7" t="s">
         <v>13</v>
@@ -5654,7 +5654,7 @@
         <v>197</v>
       </c>
       <c r="G99" s="7" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="H99" s="7"/>
       <c r="I99" s="7"/>
@@ -5688,7 +5688,7 @@
         <v>197</v>
       </c>
       <c r="G100" s="7" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="H100" s="7" t="s">
         <v>13</v>
@@ -5726,7 +5726,7 @@
         <v>234</v>
       </c>
       <c r="G101" s="7" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="H101" s="7" t="s">
         <v>12</v>
@@ -5764,7 +5764,7 @@
         <v>211</v>
       </c>
       <c r="G102" s="7" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="H102" s="7" t="s">
         <v>13</v>
@@ -5878,7 +5878,7 @@
         <v>192</v>
       </c>
       <c r="G105" s="7" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="H105" s="7" t="s">
         <v>12</v>
@@ -5916,7 +5916,7 @@
         <v>192</v>
       </c>
       <c r="G106" s="7" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="H106" s="7" t="s">
         <v>13</v>
@@ -5954,7 +5954,7 @@
         <v>208</v>
       </c>
       <c r="G107" s="7" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="H107" s="7" t="s">
         <v>12</v>
@@ -5992,7 +5992,7 @@
         <v>197</v>
       </c>
       <c r="G108" s="7" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="H108" s="7"/>
       <c r="I108" s="7"/>
@@ -6064,7 +6064,7 @@
         <v>192</v>
       </c>
       <c r="G110" s="7" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="H110" s="7" t="s">
         <v>13</v>
@@ -6102,7 +6102,7 @@
         <v>285</v>
       </c>
       <c r="G111" s="7" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="H111" s="7"/>
       <c r="I111" s="7"/>
@@ -6174,7 +6174,7 @@
         <v>234</v>
       </c>
       <c r="G113" s="7" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="H113" s="7" t="s">
         <v>13</v>
@@ -6212,7 +6212,7 @@
         <v>208</v>
       </c>
       <c r="G114" s="7" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="H114" s="7" t="s">
         <v>13</v>
@@ -6364,7 +6364,7 @@
         <v>285</v>
       </c>
       <c r="G118" s="7" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="H118" s="7"/>
       <c r="I118" s="7"/>
@@ -6398,7 +6398,7 @@
         <v>208</v>
       </c>
       <c r="G119" s="7" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="H119" s="7" t="s">
         <v>13</v>
@@ -6436,7 +6436,7 @@
         <v>211</v>
       </c>
       <c r="G120" s="7" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="H120" s="7" t="s">
         <v>12</v>
@@ -6546,7 +6546,7 @@
         <v>471</v>
       </c>
       <c r="G123" s="7" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="H123" s="7" t="s">
         <v>13</v>
@@ -6584,7 +6584,7 @@
         <v>192</v>
       </c>
       <c r="G124" s="7" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="H124" s="7"/>
       <c r="I124" s="7"/>
@@ -6618,7 +6618,7 @@
         <v>471</v>
       </c>
       <c r="G125" s="7" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="H125" s="7" t="s">
         <v>12</v>
@@ -6732,7 +6732,7 @@
         <v>188</v>
       </c>
       <c r="G128" s="7" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="H128" s="7" t="s">
         <v>13</v>
@@ -6804,7 +6804,7 @@
         <v>197</v>
       </c>
       <c r="G130" s="7" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="H130" s="7" t="s">
         <v>13</v>
@@ -6842,7 +6842,7 @@
         <v>471</v>
       </c>
       <c r="G131" s="7" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="H131" s="7"/>
       <c r="I131" s="7"/>
@@ -6952,7 +6952,7 @@
         <v>473</v>
       </c>
       <c r="G134" s="7" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="H134" s="7" t="s">
         <v>13</v>
@@ -7028,7 +7028,7 @@
         <v>474</v>
       </c>
       <c r="G136" s="7" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="H136" s="7"/>
       <c r="I136" s="7"/>
@@ -7100,7 +7100,7 @@
         <v>473</v>
       </c>
       <c r="G138" s="7" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="H138" s="7" t="s">
         <v>13</v>
@@ -7176,7 +7176,7 @@
         <v>474</v>
       </c>
       <c r="G140" s="7" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="H140" s="7" t="s">
         <v>12</v>
@@ -7364,7 +7364,7 @@
         <v>473</v>
       </c>
       <c r="G145" s="7" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="H145" s="7"/>
       <c r="I145" s="7"/>
@@ -7398,7 +7398,7 @@
         <v>473</v>
       </c>
       <c r="G146" s="7" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="H146" s="7" t="s">
         <v>13</v>
@@ -7436,7 +7436,7 @@
         <v>474</v>
       </c>
       <c r="G147" s="7" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="H147" s="7" t="s">
         <v>12</v>
@@ -7474,7 +7474,7 @@
         <v>474</v>
       </c>
       <c r="G148" s="7" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="H148" s="7" t="s">
         <v>13</v>
@@ -7548,7 +7548,7 @@
         <v>473</v>
       </c>
       <c r="G150" s="7" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="H150" s="7"/>
       <c r="I150" s="7"/>
@@ -7620,7 +7620,7 @@
         <v>474</v>
       </c>
       <c r="G152" s="7" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="H152" s="7" t="s">
         <v>12</v>
@@ -7658,7 +7658,7 @@
         <v>473</v>
       </c>
       <c r="G153" s="7" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="H153" s="7"/>
       <c r="I153" s="7"/>
@@ -7766,7 +7766,7 @@
         <v>474</v>
       </c>
       <c r="G156" s="7" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="H156" s="7"/>
       <c r="I156" s="7"/>
@@ -7838,7 +7838,7 @@
         <v>475</v>
       </c>
       <c r="G158" s="7" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="H158" s="7"/>
       <c r="I158" s="7"/>
@@ -7982,7 +7982,7 @@
         <v>475</v>
       </c>
       <c r="G162" s="7" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="H162" s="7"/>
       <c r="I162" s="7"/>
@@ -8016,7 +8016,7 @@
         <v>475</v>
       </c>
       <c r="G163" s="7" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="H163" s="7" t="s">
         <v>13</v>
@@ -8126,7 +8126,7 @@
         <v>475</v>
       </c>
       <c r="G166" s="7" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="H166" s="7"/>
       <c r="I166" s="7"/>
@@ -8160,7 +8160,7 @@
         <v>475</v>
       </c>
       <c r="G167" s="7" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="H167" s="7"/>
       <c r="I167" s="7"/>
@@ -8194,7 +8194,7 @@
         <v>475</v>
       </c>
       <c r="G168" s="7" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="H168" s="7"/>
       <c r="I168" s="7"/>

</xml_diff>